<commit_message>
Started DoorstroomData (not finished)
</commit_message>
<xml_diff>
--- a/CalculationDomain/ErasmusHogeSchool/Excels/Doorstroom 18-19.xlsx
+++ b/CalculationDomain/ErasmusHogeSchool/Excels/Doorstroom 18-19.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\jetsrv04\docentdata$\matthias.waegemans\Desktop\Cijfers instroom doorstroom\BMLT\2019\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\GIP\CalculationDomain\ErasmusHogeSchool\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70B47C30-D0B0-4FDC-B37B-AD74B7C97942}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC2476F7-D955-4E43-80F2-D50B0A7FDCAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -7584,7 +7584,7 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -7870,6 +7870,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="84.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>